<commit_message>
Penambahan 2.1.1 Survei Organisasi
Dokumen belum lengkap dan perlu dirapihkan
</commit_message>
<xml_diff>
--- a/dokumen/Jadwal.xlsx
+++ b/dokumen/Jadwal.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherenamelia/Documents/MANPRO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mardi-yuana\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF561CA-5F7E-496C-B315-FDC1830BA7E3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-960" yWindow="620" windowWidth="19600" windowHeight="15860"/>
+    <workbookView xWindow="-960" yWindow="624" windowWidth="19596" windowHeight="15864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>No/</t>
   </si>
@@ -47,9 +48,6 @@
     <t>Hari ke-</t>
   </si>
   <si>
-    <t>2,1,1</t>
-  </si>
-  <si>
     <t>2,2,1</t>
   </si>
   <si>
@@ -147,12 +145,27 @@
   </si>
   <si>
     <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Surveri Organisasi</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>1 pulpen</t>
+  </si>
+  <si>
+    <t>1 Buku tulis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -371,12 +384,43 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -387,7 +431,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -408,67 +452,83 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -752,34 +812,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:R36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="10" width="13.5" customWidth="1"/>
+    <col min="9" max="10" width="13.44140625" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="16.83203125" customWidth="1"/>
-    <col min="16" max="16" width="15.5" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" customWidth="1"/>
+    <col min="15" max="15" width="16.77734375" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -794,38 +854,38 @@
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-      <c r="Q3" s="22"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q3" s="12"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="23"/>
-    </row>
-    <row r="5" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="13"/>
+    </row>
+    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="4">
         <v>1</v>
       </c>
@@ -869,60 +929,60 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="19"/>
-    </row>
-    <row r="7" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="C6" s="16"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="24">
         <v>2.1</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
+      <c r="B7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="17"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -934,18 +994,19 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="16"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -956,16 +1017,17 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="16"/>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -978,18 +1040,19 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1000,19 +1063,20 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:18" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="19"/>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1022,20 +1086,21 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
-    </row>
-    <row r="13" spans="1:18" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>3.2</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>17</v>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29">
+        <v>3.1</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>15</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="33"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="32"/>
-      <c r="H13" s="5"/>
+      <c r="H13" s="32"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -1044,21 +1109,22 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:18" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>18</v>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29">
+        <v>3.2</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>16</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="19"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1066,36 +1132,38 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
-      <c r="R14" s="10"/>
-    </row>
-    <row r="15" spans="1:18" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>19</v>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="8"/>
+    </row>
+    <row r="15" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>17</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:18" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>4.2</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>20</v>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>18</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1103,21 +1171,22 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="17"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>4.3</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>21</v>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="29">
+        <v>4.2</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>19</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1127,419 +1196,474 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="17"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="29">
+        <v>4.3</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B19" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="34">
+        <v>5.2</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="34">
+        <v>5.3</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="34">
+        <v>5.4</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="34">
+        <v>6</v>
+      </c>
+      <c r="B25" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-    </row>
-    <row r="19" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-    </row>
-    <row r="20" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-    </row>
-    <row r="21" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>5.2</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-    </row>
-    <row r="22" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>5.3</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-    </row>
-    <row r="23" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>5.4</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-    </row>
-    <row r="24" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <v>6</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="9"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="34">
+        <v>2</v>
+      </c>
+      <c r="B26" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="13"/>
-    </row>
-    <row r="25" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <v>7</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="20"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="15"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="15"/>
-      <c r="C27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="5" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="37"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="39" t="s">
+        <v>24</v>
+      </c>
       <c r="C29" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
+      <c r="I29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P31" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>26</v>
-      </c>
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C32" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="F32" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="H32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q32" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
       <c r="C33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
+      <c r="J33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B36" s="34"/>
-      <c r="C36" t="s">
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B37" s="15"/>
+      <c r="C37" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
+  <mergeCells count="4">
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C4:P4"/>
     <mergeCell ref="C6:P6"/>
   </mergeCells>

</xml_diff>